<commit_message>
feat: remove expoport pdf and remove all nilai column
</commit_message>
<xml_diff>
--- a/public/siswa-template-import.xlsx
+++ b/public/siswa-template-import.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">nis</t>
   </si>
@@ -47,54 +47,6 @@
   </si>
   <si>
     <t xml:space="preserve">kelas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nilai1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nilai2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nilai3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nilai4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nilai5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nilai6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nilai7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nilai8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nilai9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nilai10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nilai11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nilai12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nilai13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nilai14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nilai15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nilai16</t>
   </si>
 </sst>
 </file>
@@ -383,7 +335,7 @@
   <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+      <selection pane="topLeft" activeCell="P19" activeCellId="0" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -416,54 +368,22 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>

</xml_diff>